<commit_message>
Datenbasis um Qualitäten des Personals und Bezeichnungen ergänzt
</commit_message>
<xml_diff>
--- a/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
+++ b/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>X-Wing</t>
   </si>
@@ -95,15 +95,6 @@
     <t>Personalkosten</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>***</t>
-  </si>
-  <si>
     <t>Personalkosten:</t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>Geschütz:</t>
   </si>
   <si>
-    <t>Großes Lager:</t>
-  </si>
-  <si>
     <t>Forschungsausstattung:</t>
   </si>
   <si>
@@ -156,6 +144,21 @@
   </si>
   <si>
     <t>Schulungskosten</t>
+  </si>
+  <si>
+    <t>Transportkapsel</t>
+  </si>
+  <si>
+    <t>Qualität</t>
+  </si>
+  <si>
+    <t>R2D2</t>
+  </si>
+  <si>
+    <t>Kampfdroide</t>
+  </si>
+  <si>
+    <t>Droideka</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$฿-41E]#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ [$฿-41E]_ ;_ * \-#,##0.00\ [$฿-41E]_ ;_ * &quot;-&quot;??_ [$฿-41E]_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ [$฿-41E]_ ;_ * \-#,##0.00\ [$฿-41E]_ ;_ * &quot;-&quot;??_ [$฿-41E]_ ;_ @_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -383,7 +386,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -443,13 +446,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="2" builtinId="4"/>
   </cellStyles>
@@ -758,27 +766,27 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
     <col min="12" max="12" width="31" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -794,20 +802,20 @@
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -844,7 +852,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
@@ -875,13 +883,13 @@
         <v>2</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M3" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -912,11 +920,11 @@
         <v>5</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -933,18 +941,18 @@
         <v>4000</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="40"/>
       <c r="I5" s="40"/>
       <c r="J5" s="40"/>
       <c r="L5" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -961,7 +969,7 @@
         <v>6000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" s="21">
         <v>1000</v>
@@ -978,14 +986,14 @@
         <v>10</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M6" s="24">
         <f>G10*M3+G11*M4+G12*M5</f>
         <v>45000</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1010,7 @@
         <v>5000</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" s="21">
         <v>2000</v>
@@ -1025,9 +1033,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" s="44">
         <f>G6</f>
@@ -1042,7 +1050,7 @@
         <v>3000</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G8" s="32">
         <v>3000</v>
@@ -1066,7 +1074,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -1087,10 +1095,13 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="48" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I9" s="48" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="J9" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>19</v>
@@ -1100,7 +1111,7 @@
         <v>360000</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
@@ -1117,7 +1128,7 @@
         <v>36000</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G10" s="21">
         <v>50</v>
@@ -1128,6 +1139,9 @@
       <c r="I10" s="50">
         <v>300</v>
       </c>
+      <c r="J10" s="51">
+        <v>0.9</v>
+      </c>
       <c r="L10" s="20" t="s">
         <v>17</v>
       </c>
@@ -1135,9 +1149,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F11" s="45" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G11" s="21">
         <v>100</v>
@@ -1147,6 +1161,9 @@
       </c>
       <c r="I11" s="50">
         <v>400</v>
+      </c>
+      <c r="J11" s="51">
+        <v>0.95</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>22</v>
@@ -1156,17 +1173,20 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F12" s="46" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="G12" s="32">
         <v>200</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="53">
         <v>600</v>
       </c>
-      <c r="I12" s="52"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="55">
+        <v>0.99</v>
+      </c>
       <c r="L12" s="14" t="s">
         <v>19</v>
       </c>
@@ -1175,9 +1195,9 @@
         <v>360000</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="47">
         <v>5</v>
@@ -1195,9 +1215,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B14" s="47">
         <v>300</v>
@@ -1216,7 +1236,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
       <c r="L15" s="16" t="s">
         <v>19</v>
@@ -1226,25 +1246,25 @@
         <v>360000</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L16" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M16" s="37">
         <f>M8+M11+M14</f>
         <v>2160000</v>
       </c>
     </row>
-    <row r="17" spans="10:13">
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
       <c r="L17" s="36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M17" s="30">
         <f>M6+M9+M12+M15</f>
         <v>1125000</v>
       </c>
     </row>
-    <row r="18" spans="10:13">
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
       <c r="L18" s="20" t="s">
         <v>21</v>
       </c>
@@ -1253,7 +1273,7 @@
         <v>1035000</v>
       </c>
     </row>
-    <row r="22" spans="10:13">
+    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J22" s="49"/>
     </row>
   </sheetData>
@@ -1263,7 +1283,7 @@
     <hyperlink ref="D1" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1278,7 +1298,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
@@ -1295,7 +1315,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Datenbasis Zinssatz und Zusatzkosten
</commit_message>
<xml_diff>
--- a/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
+++ b/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>X-Wing</t>
   </si>
@@ -134,12 +134,6 @@
     <t>Sonderteilkosten</t>
   </si>
   <si>
-    <t>Anzahl Pro Raumschiff</t>
-  </si>
-  <si>
-    <t>Anzahl Gesamt</t>
-  </si>
-  <si>
     <t>Werbungskosten</t>
   </si>
   <si>
@@ -159,18 +153,33 @@
   </si>
   <si>
     <t>Droideka</t>
+  </si>
+  <si>
+    <t>anfallende Zusatzkosten</t>
+  </si>
+  <si>
+    <t>anfallende Zusatzkosten in %</t>
+  </si>
+  <si>
+    <t>Zinssatz bei Überziehung in %</t>
+  </si>
+  <si>
+    <t>Anzahl Pro Raumschiff (Pers)</t>
+  </si>
+  <si>
+    <t>Anzahl Gesamt (bei Startwert)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$฿-41E]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ [$฿-41E]_ ;_ * \-#,##0.00\ [$฿-41E]_ ;_ * &quot;-&quot;??_ [$฿-41E]_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +298,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -380,16 +395,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -408,16 +444,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -455,6 +487,16 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,7 +519,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -551,7 +593,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -586,7 +627,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -762,519 +802,551 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
     <col min="12" max="12" width="31" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="5"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>18</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>38</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="19">
         <v>100</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="29">
         <f>0.6*G2</f>
         <v>60</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="29">
         <f>1.4*G2</f>
         <v>140</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="29">
         <v>1</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="22">
+      <c r="M2" s="20">
         <v>1500000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:13">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>6</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>16</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="19">
         <v>200</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="29">
         <f t="shared" ref="H3:H8" si="0">0.6*G3</f>
         <v>120</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="29">
         <f t="shared" ref="I3:I8" si="1">1.4*G3</f>
         <v>280</v>
       </c>
-      <c r="J3" s="34">
+      <c r="J3" s="29">
         <v>2</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>4</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>6</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>10</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="27">
         <v>500</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="34">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="I4" s="39">
+      <c r="I4" s="34">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="J4" s="39">
+      <c r="J4" s="34">
         <v>5</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="12"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="23">
         <f>B2*G2</f>
         <v>1800</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="23">
         <f>C2*G2</f>
         <v>3800</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="23">
         <f>D2*G2</f>
         <v>4000</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="L5" s="12" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="L5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="23">
         <f>B3*G3</f>
         <v>1200</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="23">
         <f>C3*G3</f>
         <v>3200</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <f>D3*G3</f>
         <v>6000</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <v>1000</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="35">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="35">
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="35">
         <v>10</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="22">
         <f>G10*M3+G11*M4+G12*M5</f>
         <v>45000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="37">
         <f>B4*G4</f>
         <v>2000</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="37">
         <f>C4*G4</f>
         <v>3000</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="37">
         <f>D4*G4</f>
         <v>5000</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="21">
+        <v>39</v>
+      </c>
+      <c r="G7" s="19">
         <v>2000</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="35">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="35">
         <f t="shared" si="1"/>
         <v>2800</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="35">
         <v>20</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="39">
         <f>G6</f>
         <v>1000</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="39">
         <f>G7</f>
         <v>2000</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="39">
         <f>G8</f>
         <v>3000</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="27">
         <v>3000</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="34">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="34">
         <f t="shared" si="1"/>
         <v>4200</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="34">
         <v>30</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="21">
         <f>M7*B10</f>
         <v>720000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:13">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="53">
         <f>SUM(B5:B8)</f>
         <v>6000</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="53">
         <f>SUM(C5:C8)</f>
         <v>12000</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="53">
         <f>SUM(D5:D8)</f>
         <v>18000</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="48" t="s">
+      <c r="H9" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="22">
         <f>B9*M7</f>
         <v>360000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A10" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="51">
         <f>B9*2</f>
         <v>12000</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="51">
         <f>C9*2</f>
         <v>24000</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="51">
         <f>D9*2</f>
         <v>36000</v>
       </c>
-      <c r="F10" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="21">
+      <c r="F10" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="19">
         <v>50</v>
       </c>
-      <c r="H10" s="50">
+      <c r="H10" s="45">
         <v>200</v>
       </c>
-      <c r="I10" s="50">
+      <c r="I10" s="45">
         <v>300</v>
       </c>
-      <c r="J10" s="51">
-        <v>0.9</v>
-      </c>
-      <c r="L10" s="20" t="s">
+      <c r="J10" s="46">
+        <v>0.92</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="14">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F11" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="21">
+    <row r="11" spans="1:13">
+      <c r="A11" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="55">
+        <v>15</v>
+      </c>
+      <c r="C11" s="55">
+        <v>15</v>
+      </c>
+      <c r="D11" s="55">
+        <v>15</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="19">
         <v>100</v>
       </c>
-      <c r="H11" s="50">
+      <c r="H11" s="45">
         <v>400</v>
       </c>
-      <c r="I11" s="50">
+      <c r="I11" s="45">
         <v>400</v>
       </c>
-      <c r="J11" s="51">
+      <c r="J11" s="46">
         <v>0.95</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="21">
         <f>M10*C10</f>
         <v>720000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F12" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="32">
+    <row r="12" spans="1:13">
+      <c r="A12" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="57">
+        <f>B11/100*B9</f>
+        <v>900</v>
+      </c>
+      <c r="C12" s="57">
+        <f t="shared" ref="C12:D12" si="2">C11/100*C9</f>
+        <v>1800</v>
+      </c>
+      <c r="D12" s="57">
+        <f t="shared" si="2"/>
+        <v>2700</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="27">
         <v>200</v>
       </c>
-      <c r="H12" s="53">
+      <c r="H12" s="48">
         <v>600</v>
       </c>
-      <c r="I12" s="54"/>
-      <c r="J12" s="55">
+      <c r="I12" s="49"/>
+      <c r="J12" s="50">
         <v>0.99</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="22">
         <f>C9*M10</f>
         <v>360000</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="47">
-        <v>5</v>
-      </c>
-      <c r="C13" s="47">
-        <v>10</v>
-      </c>
-      <c r="D13" s="47">
-        <v>15</v>
-      </c>
-      <c r="L13" s="20" t="s">
+    <row r="13" spans="1:13">
+      <c r="L13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="14">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="47">
-        <v>300</v>
-      </c>
-      <c r="C14" s="47">
-        <v>300</v>
-      </c>
-      <c r="D14" s="47">
-        <v>300</v>
-      </c>
-      <c r="L14" s="15" t="s">
+    <row r="14" spans="1:13">
+      <c r="L14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="21">
         <f>M13*D10</f>
         <v>720000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="2"/>
-      <c r="L15" s="16" t="s">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A15" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="42">
+        <v>5</v>
+      </c>
+      <c r="C15" s="42">
+        <v>10</v>
+      </c>
+      <c r="D15" s="42">
+        <v>15</v>
+      </c>
+      <c r="L15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="24">
         <f>D9*M13</f>
         <v>360000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L16" s="20" t="s">
+    <row r="16" spans="1:13">
+      <c r="A16" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="42">
+        <v>300</v>
+      </c>
+      <c r="C16" s="42">
+        <v>300</v>
+      </c>
+      <c r="D16" s="42">
+        <v>300</v>
+      </c>
+      <c r="L16" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="37">
+      <c r="M16" s="32">
         <f>M8+M11+M14</f>
         <v>2160000</v>
       </c>
     </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="L17" s="36" t="s">
+    <row r="17" spans="1:13">
+      <c r="L17" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="30">
+      <c r="M17" s="25">
         <f>M6+M9+M12+M15</f>
         <v>1125000</v>
       </c>
     </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="L18" s="20" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="54">
+        <v>15</v>
+      </c>
+      <c r="L18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="30">
+      <c r="M18" s="25">
         <f>M16-M17</f>
         <v>1035000</v>
       </c>
     </row>
-    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J22" s="49"/>
+    <row r="22" spans="1:13">
+      <c r="J22" s="44"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1293,12 +1365,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
@@ -1310,12 +1382,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Personal und LPE geändert in Datenbasis
</commit_message>
<xml_diff>
--- a/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
+++ b/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1251,7 @@
         <v>300</v>
       </c>
       <c r="J10" s="43">
-        <v>0.79</v>
+        <v>0.69</v>
       </c>
       <c r="L10" s="30" t="s">
         <v>36</v>
@@ -1277,7 +1277,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="11">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H11" s="42">
         <v>600</v>
@@ -1286,7 +1286,7 @@
         <v>300</v>
       </c>
       <c r="J11" s="43">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="L11" s="31" t="s">
         <v>27</v>
@@ -1316,7 +1316,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="19">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H12" s="49">
         <v>800</v>

</xml_diff>

<commit_message>
Personal laufende Kosten gestaffelt: 100, 120, 140
</commit_message>
<xml_diff>
--- a/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
+++ b/20 Spielwelt/50 Datenbasis/Datenbasis.xlsx
@@ -875,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1277,7 +1277,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="11">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H11" s="42">
         <v>600</v>
@@ -1316,7 +1316,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="19">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="H12" s="49">
         <v>800</v>

</xml_diff>